<commit_message>
Mapa atualizado com os valores das áreas.
</commit_message>
<xml_diff>
--- a/Mapa.xlsx
+++ b/Mapa.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\1Universidade\Computação Grafica\GAME3D2\Game3D\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9131A4EC-D987-4F16-8A01-D74B0C1A3B4E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A87B6998-97F8-4684-9479-6A4F63503B3E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" xr2:uid="{98500B5C-CF17-497A-8381-60AC158FEADD}"/>
   </bookViews>
@@ -171,16 +171,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>243840</xdr:colOff>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>86186</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>45162</xdr:rowOff>
+      <xdr:rowOff>51731</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>33</xdr:col>
-      <xdr:colOff>220980</xdr:colOff>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>63325</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>91440</xdr:rowOff>
+      <xdr:rowOff>98009</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -210,8 +210,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="5958840" y="593802"/>
-          <a:ext cx="4853940" cy="3703878"/>
+          <a:off x="8277686" y="603524"/>
+          <a:ext cx="4864450" cy="3724899"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -530,15 +530,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84DC1ECF-C0AB-4117-AED8-28D2D79CDD53}">
-  <dimension ref="A1:AH25"/>
+  <dimension ref="A1:AH53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J31" sqref="J31"/>
+    <sheetView tabSelected="1" zoomScale="116" workbookViewId="0">
+      <selection activeCell="AB25" sqref="AB25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="25" width="3.33203125" customWidth="1"/>
+    <col min="26" max="27" width="4.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:34" x14ac:dyDescent="0.3">
@@ -567,7 +568,13 @@
       <c r="W1" s="8"/>
       <c r="X1" s="8"/>
       <c r="Y1" s="8"/>
-      <c r="Z1" t="s">
+      <c r="Z1">
+        <v>48</v>
+      </c>
+      <c r="AA1">
+        <v>49</v>
+      </c>
+      <c r="AD1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -597,7 +604,13 @@
       <c r="W2" s="8"/>
       <c r="X2" s="8"/>
       <c r="Y2" s="8"/>
-      <c r="Z2" t="s">
+      <c r="Z2">
+        <v>46</v>
+      </c>
+      <c r="AA2">
+        <v>47</v>
+      </c>
+      <c r="AD2" t="s">
         <v>1</v>
       </c>
     </row>
@@ -627,7 +640,13 @@
       <c r="W3" s="4"/>
       <c r="X3" s="8"/>
       <c r="Y3" s="8"/>
-      <c r="Z3" t="s">
+      <c r="Z3">
+        <v>44</v>
+      </c>
+      <c r="AA3">
+        <v>45</v>
+      </c>
+      <c r="AD3" t="s">
         <v>2</v>
       </c>
     </row>
@@ -657,6 +676,12 @@
       <c r="W4" s="4"/>
       <c r="X4" s="8"/>
       <c r="Y4" s="8"/>
+      <c r="Z4">
+        <v>42</v>
+      </c>
+      <c r="AA4">
+        <v>43</v>
+      </c>
     </row>
     <row r="5" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
@@ -684,6 +709,12 @@
       <c r="W5" s="4"/>
       <c r="X5" s="8"/>
       <c r="Y5" s="8"/>
+      <c r="Z5">
+        <v>40</v>
+      </c>
+      <c r="AA5">
+        <v>41</v>
+      </c>
     </row>
     <row r="6" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
@@ -711,6 +742,12 @@
       <c r="W6" s="4"/>
       <c r="X6" s="8"/>
       <c r="Y6" s="8"/>
+      <c r="Z6">
+        <v>38</v>
+      </c>
+      <c r="AA6">
+        <v>39</v>
+      </c>
     </row>
     <row r="7" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
@@ -738,6 +775,12 @@
       <c r="W7" s="4"/>
       <c r="X7" s="8"/>
       <c r="Y7" s="8"/>
+      <c r="Z7">
+        <v>36</v>
+      </c>
+      <c r="AA7">
+        <v>37</v>
+      </c>
     </row>
     <row r="8" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
@@ -765,6 +808,12 @@
       <c r="W8" s="4"/>
       <c r="X8" s="8"/>
       <c r="Y8" s="8"/>
+      <c r="Z8">
+        <v>34</v>
+      </c>
+      <c r="AA8">
+        <v>35</v>
+      </c>
     </row>
     <row r="9" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
@@ -792,6 +841,12 @@
       <c r="W9" s="4"/>
       <c r="X9" s="8"/>
       <c r="Y9" s="8"/>
+      <c r="Z9">
+        <v>32</v>
+      </c>
+      <c r="AA9">
+        <v>33</v>
+      </c>
     </row>
     <row r="10" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
@@ -819,6 +874,12 @@
       <c r="W10" s="4"/>
       <c r="X10" s="8"/>
       <c r="Y10" s="8"/>
+      <c r="Z10">
+        <v>30</v>
+      </c>
+      <c r="AA10">
+        <v>31</v>
+      </c>
     </row>
     <row r="11" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
@@ -846,6 +907,12 @@
       <c r="W11" s="4"/>
       <c r="X11" s="8"/>
       <c r="Y11" s="8"/>
+      <c r="Z11">
+        <v>28</v>
+      </c>
+      <c r="AA11">
+        <v>29</v>
+      </c>
     </row>
     <row r="12" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
@@ -873,6 +940,12 @@
       <c r="W12" s="4"/>
       <c r="X12" s="8"/>
       <c r="Y12" s="8"/>
+      <c r="Z12">
+        <v>26</v>
+      </c>
+      <c r="AA12">
+        <v>27</v>
+      </c>
     </row>
     <row r="13" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A13" s="4"/>
@@ -900,6 +973,12 @@
       <c r="W13" s="4"/>
       <c r="X13" s="8"/>
       <c r="Y13" s="8"/>
+      <c r="Z13">
+        <v>24</v>
+      </c>
+      <c r="AA13">
+        <v>25</v>
+      </c>
     </row>
     <row r="14" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A14" s="8"/>
@@ -927,6 +1006,12 @@
       <c r="W14" s="4"/>
       <c r="X14" s="8"/>
       <c r="Y14" s="8"/>
+      <c r="Z14">
+        <v>22</v>
+      </c>
+      <c r="AA14">
+        <v>23</v>
+      </c>
     </row>
     <row r="15" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A15" s="8"/>
@@ -954,6 +1039,12 @@
       <c r="W15" s="4"/>
       <c r="X15" s="8"/>
       <c r="Y15" s="8"/>
+      <c r="Z15">
+        <v>20</v>
+      </c>
+      <c r="AA15">
+        <v>21</v>
+      </c>
     </row>
     <row r="16" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
@@ -981,9 +1072,15 @@
       <c r="W16" s="4"/>
       <c r="X16" s="8"/>
       <c r="Y16" s="8"/>
+      <c r="Z16">
+        <v>18</v>
+      </c>
+      <c r="AA16">
+        <v>19</v>
+      </c>
       <c r="AH16" s="9"/>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
@@ -1009,8 +1106,14 @@
       <c r="W17" s="4"/>
       <c r="X17" s="8"/>
       <c r="Y17" s="8"/>
-    </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z17">
+        <v>16</v>
+      </c>
+      <c r="AA17">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
@@ -1036,8 +1139,14 @@
       <c r="W18" s="4"/>
       <c r="X18" s="8"/>
       <c r="Y18" s="8"/>
-    </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z18">
+        <v>14</v>
+      </c>
+      <c r="AA18">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
@@ -1063,8 +1172,14 @@
       <c r="W19" s="4"/>
       <c r="X19" s="8"/>
       <c r="Y19" s="8"/>
-    </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z19">
+        <v>12</v>
+      </c>
+      <c r="AA19">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A20" s="8"/>
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
@@ -1090,8 +1205,14 @@
       <c r="W20" s="4"/>
       <c r="X20" s="8"/>
       <c r="Y20" s="8"/>
-    </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z20">
+        <v>10</v>
+      </c>
+      <c r="AA20">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A21" s="8"/>
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>
@@ -1117,8 +1238,14 @@
       <c r="W21" s="4"/>
       <c r="X21" s="8"/>
       <c r="Y21" s="8"/>
-    </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z21">
+        <v>8</v>
+      </c>
+      <c r="AA21">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A22" s="8"/>
       <c r="B22" s="8"/>
       <c r="K22" s="8"/>
@@ -1136,8 +1263,14 @@
       <c r="W22" s="8"/>
       <c r="X22" s="8"/>
       <c r="Y22" s="8"/>
-    </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z22">
+        <v>6</v>
+      </c>
+      <c r="AA22">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A23" s="8"/>
       <c r="B23" s="8"/>
       <c r="D23" s="4"/>
@@ -1162,8 +1295,14 @@
       <c r="W23" s="8"/>
       <c r="X23" s="8"/>
       <c r="Y23" s="8"/>
-    </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z23">
+        <v>4</v>
+      </c>
+      <c r="AA23">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A24" s="8"/>
       <c r="B24" s="8"/>
       <c r="D24" s="4"/>
@@ -1188,8 +1327,14 @@
       <c r="W24" s="4"/>
       <c r="X24" s="4"/>
       <c r="Y24" s="5"/>
-    </row>
-    <row r="25" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="Z24">
+        <v>2</v>
+      </c>
+      <c r="AA24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="8"/>
       <c r="B25" s="8"/>
       <c r="C25" s="6"/>
@@ -1215,6 +1360,833 @@
       <c r="W25" s="6"/>
       <c r="X25" s="6"/>
       <c r="Y25" s="7"/>
+      <c r="Z25">
+        <v>0</v>
+      </c>
+      <c r="AA25">
+        <v>1</v>
+      </c>
+      <c r="AB25" s="9"/>
+    </row>
+    <row r="26" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>0</v>
+      </c>
+      <c r="B26">
+        <v>2</v>
+      </c>
+      <c r="C26">
+        <v>4</v>
+      </c>
+      <c r="D26">
+        <v>6</v>
+      </c>
+      <c r="E26">
+        <v>8</v>
+      </c>
+      <c r="F26">
+        <v>10</v>
+      </c>
+      <c r="G26">
+        <v>12</v>
+      </c>
+      <c r="H26">
+        <v>14</v>
+      </c>
+      <c r="I26">
+        <v>16</v>
+      </c>
+      <c r="J26">
+        <v>18</v>
+      </c>
+      <c r="K26">
+        <v>20</v>
+      </c>
+      <c r="L26">
+        <v>22</v>
+      </c>
+      <c r="M26">
+        <v>24</v>
+      </c>
+      <c r="N26">
+        <v>26</v>
+      </c>
+      <c r="O26">
+        <v>28</v>
+      </c>
+      <c r="P26">
+        <v>30</v>
+      </c>
+      <c r="Q26">
+        <v>32</v>
+      </c>
+      <c r="R26">
+        <v>34</v>
+      </c>
+      <c r="S26">
+        <v>36</v>
+      </c>
+      <c r="T26">
+        <v>38</v>
+      </c>
+      <c r="U26">
+        <v>40</v>
+      </c>
+      <c r="V26">
+        <v>42</v>
+      </c>
+      <c r="W26">
+        <v>44</v>
+      </c>
+      <c r="X26">
+        <v>46</v>
+      </c>
+      <c r="Y26">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="27" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>1</v>
+      </c>
+      <c r="B27">
+        <v>3</v>
+      </c>
+      <c r="C27">
+        <v>5</v>
+      </c>
+      <c r="D27">
+        <v>7</v>
+      </c>
+      <c r="E27">
+        <v>9</v>
+      </c>
+      <c r="F27">
+        <v>11</v>
+      </c>
+      <c r="G27">
+        <v>13</v>
+      </c>
+      <c r="H27">
+        <v>15</v>
+      </c>
+      <c r="I27">
+        <v>17</v>
+      </c>
+      <c r="J27">
+        <v>19</v>
+      </c>
+      <c r="K27">
+        <v>21</v>
+      </c>
+      <c r="L27">
+        <v>23</v>
+      </c>
+      <c r="M27">
+        <v>25</v>
+      </c>
+      <c r="N27">
+        <v>27</v>
+      </c>
+      <c r="O27">
+        <v>29</v>
+      </c>
+      <c r="P27">
+        <v>31</v>
+      </c>
+      <c r="Q27">
+        <v>33</v>
+      </c>
+      <c r="R27">
+        <v>35</v>
+      </c>
+      <c r="S27">
+        <v>37</v>
+      </c>
+      <c r="T27">
+        <v>39</v>
+      </c>
+      <c r="U27">
+        <v>41</v>
+      </c>
+      <c r="V27">
+        <v>43</v>
+      </c>
+      <c r="W27">
+        <v>45</v>
+      </c>
+      <c r="X27">
+        <v>47</v>
+      </c>
+      <c r="Y27">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="28" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="29" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A29" s="1"/>
+      <c r="B29" s="8"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="8"/>
+      <c r="L29" s="8"/>
+      <c r="M29" s="8"/>
+      <c r="N29" s="8"/>
+      <c r="O29" s="8"/>
+      <c r="P29" s="8"/>
+      <c r="Q29" s="8"/>
+      <c r="R29" s="8"/>
+      <c r="S29" s="8"/>
+      <c r="T29" s="8"/>
+      <c r="U29" s="8"/>
+      <c r="V29" s="8"/>
+      <c r="W29" s="8"/>
+      <c r="X29" s="8"/>
+      <c r="Y29" s="8"/>
+    </row>
+    <row r="30" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A30" s="3"/>
+      <c r="B30" s="8"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4"/>
+      <c r="I30" s="4"/>
+      <c r="J30" s="4"/>
+      <c r="K30" s="8"/>
+      <c r="L30" s="8"/>
+      <c r="M30" s="8"/>
+      <c r="N30" s="8"/>
+      <c r="O30" s="8"/>
+      <c r="P30" s="8"/>
+      <c r="Q30" s="8"/>
+      <c r="R30" s="8"/>
+      <c r="S30" s="8"/>
+      <c r="T30" s="8"/>
+      <c r="U30" s="8"/>
+      <c r="V30" s="8"/>
+      <c r="W30" s="8"/>
+      <c r="X30" s="8"/>
+      <c r="Y30" s="8"/>
+    </row>
+    <row r="31" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A31" s="3"/>
+      <c r="B31" s="8"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
+      <c r="H31" s="4"/>
+      <c r="I31" s="4"/>
+      <c r="J31" s="4"/>
+      <c r="K31" s="8"/>
+      <c r="L31" s="8"/>
+      <c r="M31" s="4"/>
+      <c r="N31" s="4"/>
+      <c r="O31" s="4"/>
+      <c r="P31" s="4"/>
+      <c r="Q31" s="4"/>
+      <c r="R31" s="4"/>
+      <c r="S31" s="4"/>
+      <c r="T31" s="4"/>
+      <c r="U31" s="4"/>
+      <c r="V31" s="4"/>
+      <c r="W31" s="4"/>
+      <c r="X31" s="8"/>
+      <c r="Y31" s="8"/>
+    </row>
+    <row r="32" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A32" s="3"/>
+      <c r="B32" s="8"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="4"/>
+      <c r="I32" s="4"/>
+      <c r="J32" s="4"/>
+      <c r="K32" s="8"/>
+      <c r="L32" s="8"/>
+      <c r="M32" s="4"/>
+      <c r="N32" s="4"/>
+      <c r="O32" s="4"/>
+      <c r="P32" s="4"/>
+      <c r="Q32" s="4"/>
+      <c r="R32" s="4"/>
+      <c r="S32" s="4"/>
+      <c r="T32" s="4"/>
+      <c r="U32" s="4"/>
+      <c r="V32" s="4"/>
+      <c r="W32" s="4"/>
+      <c r="X32" s="8"/>
+      <c r="Y32" s="8"/>
+    </row>
+    <row r="33" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A33" s="3"/>
+      <c r="B33" s="8"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="8"/>
+      <c r="F33" s="8"/>
+      <c r="G33" s="8"/>
+      <c r="H33" s="4"/>
+      <c r="I33" s="4"/>
+      <c r="J33" s="4"/>
+      <c r="K33" s="8"/>
+      <c r="L33" s="8"/>
+      <c r="M33" s="8"/>
+      <c r="N33" s="8"/>
+      <c r="O33" s="8"/>
+      <c r="P33" s="8"/>
+      <c r="Q33" s="8"/>
+      <c r="R33" s="8"/>
+      <c r="S33" s="8"/>
+      <c r="T33" s="4"/>
+      <c r="U33" s="4"/>
+      <c r="V33" s="4"/>
+      <c r="W33" s="4"/>
+      <c r="X33" s="8"/>
+      <c r="Y33" s="8"/>
+    </row>
+    <row r="34" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A34" s="3"/>
+      <c r="B34" s="8"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="8"/>
+      <c r="E34" s="8"/>
+      <c r="F34" s="8"/>
+      <c r="G34" s="8"/>
+      <c r="H34" s="8"/>
+      <c r="I34" s="8"/>
+      <c r="J34" s="8"/>
+      <c r="K34" s="8"/>
+      <c r="L34" s="8"/>
+      <c r="M34" s="8"/>
+      <c r="N34" s="8"/>
+      <c r="O34" s="8"/>
+      <c r="P34" s="8"/>
+      <c r="Q34" s="8"/>
+      <c r="R34" s="8"/>
+      <c r="S34" s="8"/>
+      <c r="T34" s="4"/>
+      <c r="U34" s="4"/>
+      <c r="V34" s="4"/>
+      <c r="W34" s="4"/>
+      <c r="X34" s="8"/>
+      <c r="Y34" s="8"/>
+    </row>
+    <row r="35" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A35" s="3"/>
+      <c r="B35" s="8"/>
+      <c r="C35" s="8"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="8"/>
+      <c r="G35" s="8"/>
+      <c r="H35" s="8"/>
+      <c r="I35" s="8"/>
+      <c r="J35" s="8"/>
+      <c r="K35" s="8"/>
+      <c r="L35" s="8"/>
+      <c r="M35" s="4"/>
+      <c r="N35" s="4"/>
+      <c r="O35" s="8"/>
+      <c r="P35" s="8"/>
+      <c r="Q35" s="4"/>
+      <c r="R35" s="8"/>
+      <c r="S35" s="8"/>
+      <c r="T35" s="4"/>
+      <c r="U35" s="4"/>
+      <c r="V35" s="4"/>
+      <c r="W35" s="4"/>
+      <c r="X35" s="8"/>
+      <c r="Y35" s="8"/>
+    </row>
+    <row r="36" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A36" s="3"/>
+      <c r="B36" s="8"/>
+      <c r="C36" s="8"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="8"/>
+      <c r="G36" s="8"/>
+      <c r="H36" s="4"/>
+      <c r="I36" s="4"/>
+      <c r="J36" s="4"/>
+      <c r="K36" s="8"/>
+      <c r="L36" s="8"/>
+      <c r="M36" s="4"/>
+      <c r="N36" s="4"/>
+      <c r="O36" s="8"/>
+      <c r="P36" s="8"/>
+      <c r="Q36" s="4"/>
+      <c r="R36" s="8"/>
+      <c r="S36" s="8"/>
+      <c r="T36" s="4"/>
+      <c r="U36" s="4"/>
+      <c r="V36" s="4"/>
+      <c r="W36" s="4"/>
+      <c r="X36" s="8"/>
+      <c r="Y36" s="8"/>
+    </row>
+    <row r="37" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A37" s="3"/>
+      <c r="B37" s="8"/>
+      <c r="C37" s="8"/>
+      <c r="D37" s="8"/>
+      <c r="E37" s="8"/>
+      <c r="F37" s="8"/>
+      <c r="G37" s="8"/>
+      <c r="H37" s="4"/>
+      <c r="I37" s="4"/>
+      <c r="J37" s="4"/>
+      <c r="K37" s="8"/>
+      <c r="L37" s="8"/>
+      <c r="M37" s="4"/>
+      <c r="N37" s="4"/>
+      <c r="O37" s="8"/>
+      <c r="P37" s="8"/>
+      <c r="Q37" s="4"/>
+      <c r="R37" s="8"/>
+      <c r="S37" s="8"/>
+      <c r="T37" s="4"/>
+      <c r="U37" s="4"/>
+      <c r="V37" s="4"/>
+      <c r="W37" s="4"/>
+      <c r="X37" s="8"/>
+      <c r="Y37" s="8"/>
+    </row>
+    <row r="38" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A38" s="3"/>
+      <c r="B38" s="8"/>
+      <c r="C38" s="8"/>
+      <c r="D38" s="8"/>
+      <c r="E38" s="8"/>
+      <c r="F38" s="8"/>
+      <c r="G38" s="8"/>
+      <c r="H38" s="4"/>
+      <c r="I38" s="4"/>
+      <c r="J38" s="4"/>
+      <c r="K38" s="8"/>
+      <c r="L38" s="8"/>
+      <c r="M38" s="4"/>
+      <c r="N38" s="4"/>
+      <c r="O38" s="8"/>
+      <c r="P38" s="8"/>
+      <c r="Q38" s="4"/>
+      <c r="R38" s="8"/>
+      <c r="S38" s="8"/>
+      <c r="T38" s="4"/>
+      <c r="U38" s="4"/>
+      <c r="V38" s="4"/>
+      <c r="W38" s="4"/>
+      <c r="X38" s="8"/>
+      <c r="Y38" s="8"/>
+    </row>
+    <row r="39" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A39" s="3"/>
+      <c r="B39" s="4"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="8"/>
+      <c r="G39" s="8"/>
+      <c r="H39" s="4"/>
+      <c r="I39" s="4"/>
+      <c r="J39" s="4"/>
+      <c r="K39" s="8"/>
+      <c r="L39" s="8"/>
+      <c r="M39" s="4"/>
+      <c r="N39" s="8"/>
+      <c r="O39" s="8"/>
+      <c r="P39" s="8"/>
+      <c r="Q39" s="8"/>
+      <c r="R39" s="8"/>
+      <c r="S39" s="8"/>
+      <c r="T39" s="4"/>
+      <c r="U39" s="4"/>
+      <c r="V39" s="4"/>
+      <c r="W39" s="4"/>
+      <c r="X39" s="8"/>
+      <c r="Y39" s="8"/>
+    </row>
+    <row r="40" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A40" s="3"/>
+      <c r="B40" s="4"/>
+      <c r="C40" s="4"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="8"/>
+      <c r="G40" s="8"/>
+      <c r="H40" s="4"/>
+      <c r="I40" s="4"/>
+      <c r="J40" s="4"/>
+      <c r="K40" s="8"/>
+      <c r="L40" s="8"/>
+      <c r="M40" s="4"/>
+      <c r="N40" s="8"/>
+      <c r="O40" s="8"/>
+      <c r="P40" s="8"/>
+      <c r="Q40" s="8"/>
+      <c r="R40" s="8"/>
+      <c r="S40" s="8"/>
+      <c r="T40" s="4"/>
+      <c r="U40" s="4"/>
+      <c r="V40" s="4"/>
+      <c r="W40" s="4"/>
+      <c r="X40" s="8"/>
+      <c r="Y40" s="8"/>
+    </row>
+    <row r="41" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A41" s="4"/>
+      <c r="B41" s="4"/>
+      <c r="C41" s="4"/>
+      <c r="D41" s="4"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="8"/>
+      <c r="G41" s="8"/>
+      <c r="H41" s="4"/>
+      <c r="I41" s="4"/>
+      <c r="J41" s="4"/>
+      <c r="K41" s="8"/>
+      <c r="L41" s="8"/>
+      <c r="M41" s="4"/>
+      <c r="N41" s="8"/>
+      <c r="O41" s="8"/>
+      <c r="P41" s="4"/>
+      <c r="Q41" s="4"/>
+      <c r="R41" s="8"/>
+      <c r="S41" s="8"/>
+      <c r="T41" s="4"/>
+      <c r="U41" s="4"/>
+      <c r="V41" s="4"/>
+      <c r="W41" s="4"/>
+      <c r="X41" s="8"/>
+      <c r="Y41" s="8"/>
+    </row>
+    <row r="42" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A42" s="8"/>
+      <c r="B42" s="8"/>
+      <c r="C42" s="8"/>
+      <c r="D42" s="8"/>
+      <c r="E42" s="8"/>
+      <c r="F42" s="8"/>
+      <c r="G42" s="8"/>
+      <c r="H42" s="8"/>
+      <c r="I42" s="8"/>
+      <c r="J42" s="8"/>
+      <c r="K42" s="8"/>
+      <c r="L42" s="8"/>
+      <c r="M42" s="8"/>
+      <c r="N42" s="8"/>
+      <c r="O42" s="8"/>
+      <c r="P42" s="4"/>
+      <c r="Q42" s="4"/>
+      <c r="R42" s="8"/>
+      <c r="S42" s="8"/>
+      <c r="T42" s="4"/>
+      <c r="U42" s="4"/>
+      <c r="V42" s="4"/>
+      <c r="W42" s="4"/>
+      <c r="X42" s="8"/>
+      <c r="Y42" s="8"/>
+    </row>
+    <row r="43" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A43" s="8"/>
+      <c r="B43" s="8"/>
+      <c r="C43" s="8"/>
+      <c r="D43" s="8"/>
+      <c r="E43" s="8"/>
+      <c r="F43" s="8"/>
+      <c r="G43" s="8"/>
+      <c r="H43" s="8"/>
+      <c r="I43" s="8"/>
+      <c r="J43" s="8"/>
+      <c r="K43" s="8"/>
+      <c r="L43" s="8"/>
+      <c r="M43" s="8"/>
+      <c r="N43" s="8"/>
+      <c r="O43" s="8"/>
+      <c r="P43" s="4"/>
+      <c r="Q43" s="4"/>
+      <c r="R43" s="8"/>
+      <c r="S43" s="8"/>
+      <c r="T43" s="4"/>
+      <c r="U43" s="4"/>
+      <c r="V43" s="4"/>
+      <c r="W43" s="4"/>
+      <c r="X43" s="8"/>
+      <c r="Y43" s="8"/>
+    </row>
+    <row r="44" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A44" s="3"/>
+      <c r="B44" s="4"/>
+      <c r="C44" s="4"/>
+      <c r="D44" s="4"/>
+      <c r="E44" s="8"/>
+      <c r="F44" s="8"/>
+      <c r="G44" s="4"/>
+      <c r="H44" s="4"/>
+      <c r="I44" s="4"/>
+      <c r="J44" s="4"/>
+      <c r="K44" s="8"/>
+      <c r="L44" s="8"/>
+      <c r="M44" s="4"/>
+      <c r="N44" s="4"/>
+      <c r="O44" s="4"/>
+      <c r="P44" s="4"/>
+      <c r="Q44" s="4"/>
+      <c r="R44" s="8"/>
+      <c r="S44" s="8"/>
+      <c r="T44" s="4"/>
+      <c r="U44" s="4"/>
+      <c r="V44" s="4"/>
+      <c r="W44" s="4"/>
+      <c r="X44" s="8"/>
+      <c r="Y44" s="8"/>
+    </row>
+    <row r="45" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A45" s="3"/>
+      <c r="B45" s="4"/>
+      <c r="C45" s="4"/>
+      <c r="D45" s="4"/>
+      <c r="E45" s="8"/>
+      <c r="F45" s="8"/>
+      <c r="G45" s="4"/>
+      <c r="H45" s="4"/>
+      <c r="I45" s="4"/>
+      <c r="J45" s="4"/>
+      <c r="K45" s="8"/>
+      <c r="L45" s="8"/>
+      <c r="M45" s="8"/>
+      <c r="N45" s="8"/>
+      <c r="O45" s="8"/>
+      <c r="P45" s="8"/>
+      <c r="Q45" s="8"/>
+      <c r="R45" s="8"/>
+      <c r="S45" s="8"/>
+      <c r="T45" s="4"/>
+      <c r="U45" s="4"/>
+      <c r="V45" s="4"/>
+      <c r="W45" s="4"/>
+      <c r="X45" s="8"/>
+      <c r="Y45" s="8"/>
+    </row>
+    <row r="46" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A46" s="3"/>
+      <c r="B46" s="4"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="4"/>
+      <c r="E46" s="8"/>
+      <c r="F46" s="8"/>
+      <c r="G46" s="4"/>
+      <c r="H46" s="4"/>
+      <c r="I46" s="4"/>
+      <c r="J46" s="4"/>
+      <c r="K46" s="8"/>
+      <c r="L46" s="8"/>
+      <c r="M46" s="8"/>
+      <c r="N46" s="8"/>
+      <c r="O46" s="8"/>
+      <c r="P46" s="8"/>
+      <c r="Q46" s="8"/>
+      <c r="R46" s="8"/>
+      <c r="S46" s="8"/>
+      <c r="T46" s="4"/>
+      <c r="U46" s="4"/>
+      <c r="V46" s="4"/>
+      <c r="W46" s="4"/>
+      <c r="X46" s="8"/>
+      <c r="Y46" s="8"/>
+    </row>
+    <row r="47" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A47" s="3"/>
+      <c r="B47" s="4"/>
+      <c r="C47" s="4"/>
+      <c r="D47" s="4"/>
+      <c r="E47" s="8"/>
+      <c r="F47" s="8"/>
+      <c r="G47" s="4"/>
+      <c r="H47" s="4"/>
+      <c r="I47" s="4"/>
+      <c r="J47" s="4"/>
+      <c r="K47" s="8"/>
+      <c r="L47" s="8"/>
+      <c r="M47" s="4"/>
+      <c r="N47" s="4"/>
+      <c r="O47" s="4"/>
+      <c r="P47" s="4"/>
+      <c r="Q47" s="4"/>
+      <c r="R47" s="8"/>
+      <c r="S47" s="8"/>
+      <c r="T47" s="4"/>
+      <c r="U47" s="4"/>
+      <c r="V47" s="4"/>
+      <c r="W47" s="4"/>
+      <c r="X47" s="8"/>
+      <c r="Y47" s="8"/>
+    </row>
+    <row r="48" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A48" s="8"/>
+      <c r="B48" s="8"/>
+      <c r="C48" s="8"/>
+      <c r="D48" s="8"/>
+      <c r="E48" s="8"/>
+      <c r="F48" s="8"/>
+      <c r="G48" s="8"/>
+      <c r="H48" s="8"/>
+      <c r="I48" s="8"/>
+      <c r="J48" s="8"/>
+      <c r="K48" s="8"/>
+      <c r="L48" s="8"/>
+      <c r="M48" s="4"/>
+      <c r="N48" s="4"/>
+      <c r="O48" s="4"/>
+      <c r="P48" s="4"/>
+      <c r="Q48" s="4"/>
+      <c r="R48" s="8"/>
+      <c r="S48" s="8"/>
+      <c r="T48" s="4"/>
+      <c r="U48" s="4"/>
+      <c r="V48" s="4"/>
+      <c r="W48" s="4"/>
+      <c r="X48" s="8"/>
+      <c r="Y48" s="8"/>
+    </row>
+    <row r="49" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A49" s="8"/>
+      <c r="B49" s="8"/>
+      <c r="C49" s="8"/>
+      <c r="D49" s="8"/>
+      <c r="E49" s="8"/>
+      <c r="F49" s="8"/>
+      <c r="G49" s="8"/>
+      <c r="H49" s="8"/>
+      <c r="I49" s="8"/>
+      <c r="J49" s="8"/>
+      <c r="K49" s="8"/>
+      <c r="L49" s="8"/>
+      <c r="M49" s="4"/>
+      <c r="N49" s="4"/>
+      <c r="O49" s="4"/>
+      <c r="P49" s="4"/>
+      <c r="Q49" s="4"/>
+      <c r="R49" s="8"/>
+      <c r="S49" s="8"/>
+      <c r="T49" s="4"/>
+      <c r="U49" s="4"/>
+      <c r="V49" s="4"/>
+      <c r="W49" s="4"/>
+      <c r="X49" s="8"/>
+      <c r="Y49" s="8"/>
+    </row>
+    <row r="50" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A50" s="8"/>
+      <c r="B50" s="8"/>
+      <c r="K50" s="8"/>
+      <c r="L50" s="8"/>
+      <c r="M50" s="8"/>
+      <c r="N50" s="8"/>
+      <c r="O50" s="8"/>
+      <c r="P50" s="8"/>
+      <c r="Q50" s="8"/>
+      <c r="R50" s="8"/>
+      <c r="S50" s="8"/>
+      <c r="T50" s="8"/>
+      <c r="U50" s="8"/>
+      <c r="V50" s="8"/>
+      <c r="W50" s="8"/>
+      <c r="X50" s="8"/>
+      <c r="Y50" s="8"/>
+    </row>
+    <row r="51" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A51" s="8"/>
+      <c r="B51" s="8"/>
+      <c r="D51" s="4"/>
+      <c r="E51" s="4"/>
+      <c r="F51" s="4"/>
+      <c r="G51" s="4"/>
+      <c r="H51" s="4"/>
+      <c r="I51" s="4"/>
+      <c r="J51" s="4"/>
+      <c r="K51" s="8"/>
+      <c r="L51" s="8"/>
+      <c r="M51" s="8"/>
+      <c r="N51" s="8"/>
+      <c r="O51" s="8"/>
+      <c r="P51" s="8"/>
+      <c r="Q51" s="8"/>
+      <c r="R51" s="8"/>
+      <c r="S51" s="8"/>
+      <c r="T51" s="8"/>
+      <c r="U51" s="8"/>
+      <c r="V51" s="8"/>
+      <c r="W51" s="8"/>
+      <c r="X51" s="8"/>
+      <c r="Y51" s="8"/>
+    </row>
+    <row r="52" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A52" s="8"/>
+      <c r="B52" s="8"/>
+      <c r="D52" s="4"/>
+      <c r="E52" s="4"/>
+      <c r="F52" s="4"/>
+      <c r="G52" s="4"/>
+      <c r="H52" s="4"/>
+      <c r="I52" s="4"/>
+      <c r="J52" s="4"/>
+      <c r="K52" s="8"/>
+      <c r="L52" s="8"/>
+      <c r="M52" s="4"/>
+      <c r="N52" s="4"/>
+      <c r="O52" s="4"/>
+      <c r="P52" s="4"/>
+      <c r="Q52" s="4"/>
+      <c r="R52" s="4"/>
+      <c r="S52" s="4"/>
+      <c r="T52" s="4"/>
+      <c r="U52" s="4"/>
+      <c r="V52" s="4"/>
+      <c r="W52" s="4"/>
+      <c r="X52" s="4"/>
+      <c r="Y52" s="5"/>
+    </row>
+    <row r="53" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="8"/>
+      <c r="B53" s="8"/>
+      <c r="C53" s="6"/>
+      <c r="D53" s="6"/>
+      <c r="E53" s="6"/>
+      <c r="F53" s="6"/>
+      <c r="G53" s="6"/>
+      <c r="H53" s="6"/>
+      <c r="I53" s="6"/>
+      <c r="J53" s="6"/>
+      <c r="K53" s="8"/>
+      <c r="L53" s="8"/>
+      <c r="M53" s="6"/>
+      <c r="N53" s="6"/>
+      <c r="O53" s="6"/>
+      <c r="P53" s="6"/>
+      <c r="Q53" s="6"/>
+      <c r="R53" s="6"/>
+      <c r="S53" s="6"/>
+      <c r="T53" s="6"/>
+      <c r="U53" s="6"/>
+      <c r="V53" s="6"/>
+      <c r="W53" s="6"/>
+      <c r="X53" s="6"/>
+      <c r="Y53" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>